<commit_message>
Adjustments of the distribution plot
</commit_message>
<xml_diff>
--- a/screening/screening_books-chapter_done.xlsx
+++ b/screening/screening_books-chapter_done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoffmanka/Documents/dev/smart-on-fhir-literature-research/smart-on-fhir-literature-analysis/screening/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3597628-DBCF-E045-BC49-1C1032A16106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1C0063-DEA8-8D44-A42E-4850F0B40204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1561,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M43" workbookViewId="0">
-      <selection activeCell="T61" sqref="T61"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R61" sqref="R61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Working on concatinate the individual screening files and prepare the final analysis
</commit_message>
<xml_diff>
--- a/screening/screening_books-chapter_done.xlsx
+++ b/screening/screening_books-chapter_done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoffmanka/Documents/dev/smart-on-fhir-literature-research/smart-on-fhir-literature-analysis/screening/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1C0063-DEA8-8D44-A42E-4850F0B40204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5653880C-F2D1-4B4B-87A7-FB2A8CCF268A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="369">
   <si>
     <t>id</t>
   </si>
@@ -1117,9 +1117,6 @@
     <t>no reference implementation</t>
   </si>
   <si>
-    <t>Fulltext</t>
-  </si>
-  <si>
     <t>no access</t>
   </si>
   <si>
@@ -1139,6 +1136,12 @@
   </si>
   <si>
     <t>brief introduction</t>
+  </si>
+  <si>
+    <t>further excluded</t>
+  </si>
+  <si>
+    <t>Fulltext screening</t>
   </si>
 </sst>
 </file>
@@ -1157,6 +1160,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1172,7 +1176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1200,6 +1204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,7 +1252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1252,11 +1262,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1559,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R61" sqref="R61"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1572,10 +1584,11 @@
     <col min="17" max="17" width="4.83203125" customWidth="1"/>
     <col min="18" max="18" width="9.83203125" customWidth="1"/>
     <col min="19" max="19" width="67.1640625" customWidth="1"/>
-    <col min="20" max="20" width="23.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1633,11 +1646,14 @@
       <c r="S1" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T1" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1678,11 +1694,14 @@
         <v>1</v>
       </c>
       <c r="S2" s="3"/>
-      <c r="T2" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T2" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1722,8 +1741,10 @@
       <c r="S3" s="3" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T3" s="5"/>
+      <c r="U3" s="7"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1763,58 +1784,61 @@
       <c r="S4" s="3" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="T4" s="5"/>
+      <c r="U4" s="7"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>2018</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>43</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7" t="s">
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7">
+      <c r="P5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
         <v>1</v>
       </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S5" s="6"/>
+      <c r="T5" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="U5" s="7"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1852,11 +1876,14 @@
         <v>1</v>
       </c>
       <c r="S6" s="3"/>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="5" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1896,8 +1923,10 @@
       <c r="S7" s="3" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T7" s="5"/>
+      <c r="U7" s="7"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1935,11 +1964,14 @@
         <v>1</v>
       </c>
       <c r="S8" s="3"/>
-      <c r="T8" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T8" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1977,11 +2009,14 @@
         <v>1</v>
       </c>
       <c r="S9" s="3"/>
-      <c r="T9" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T9" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2021,8 +2056,10 @@
       <c r="S10" s="3" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T10" s="5"/>
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2065,8 +2102,10 @@
       <c r="S11" s="3" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T11" s="5"/>
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2106,8 +2145,10 @@
       <c r="S12" s="3" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T12" s="5"/>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2150,8 +2191,10 @@
       <c r="S13" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T13" s="5"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2192,11 +2235,14 @@
         <v>1</v>
       </c>
       <c r="S14" s="3"/>
-      <c r="T14" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T14" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2237,61 +2283,65 @@
         <v>1</v>
       </c>
       <c r="S15" s="3"/>
-      <c r="T15" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="T15" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>2022</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7" t="s">
+      <c r="J16" s="6"/>
+      <c r="K16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7">
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6">
         <v>1</v>
       </c>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S16" s="6"/>
+      <c r="T16" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2329,11 +2379,14 @@
         <v>1</v>
       </c>
       <c r="S17" s="3"/>
-      <c r="T17" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T17" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2370,8 +2423,10 @@
       <c r="S18" s="3" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T18" s="5"/>
+      <c r="U18" s="7"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2411,8 +2466,10 @@
       <c r="S19" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T19" s="5"/>
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2452,58 +2509,61 @@
       <c r="S20" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
+      <c r="T20" s="5"/>
+      <c r="U20" s="7"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>2022</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7" t="s">
+      <c r="J21" s="6"/>
+      <c r="K21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7">
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6">
         <v>1</v>
       </c>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S21" s="6"/>
+      <c r="T21" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="U21" s="7"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2546,8 +2606,10 @@
       <c r="S22" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T22" s="5"/>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2584,8 +2646,10 @@
       <c r="S23" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T23" s="5"/>
+      <c r="U23" s="7"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2626,11 +2690,14 @@
         <v>1</v>
       </c>
       <c r="S24" s="3"/>
-      <c r="T24" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T24" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2670,8 +2737,10 @@
       <c r="S25" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T25" s="5"/>
+      <c r="U25" s="7"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2712,11 +2781,14 @@
         <v>1</v>
       </c>
       <c r="S26" s="3"/>
-      <c r="T26" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T26" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U26" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2757,11 +2829,14 @@
         <v>1</v>
       </c>
       <c r="S27" s="3"/>
-      <c r="T27" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T27" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2804,11 +2879,10 @@
       <c r="S28" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="T28" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T28" s="5"/>
+      <c r="U28" s="7"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2848,8 +2922,10 @@
       <c r="S29" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T29" s="5"/>
+      <c r="U29" s="7"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2892,54 +2968,57 @@
       <c r="S30" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
+      <c r="T30" s="5"/>
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
         <v>29</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>2017</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>1</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7" t="s">
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7">
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6">
         <v>1</v>
       </c>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S31" s="6"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="7"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2980,11 +3059,14 @@
         <v>1</v>
       </c>
       <c r="S32" s="4"/>
-      <c r="T32" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T32" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U32" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3027,8 +3109,10 @@
       <c r="S33" s="3" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T33" s="5"/>
+      <c r="U33" s="7"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3065,8 +3149,10 @@
       <c r="S34" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T34" s="5"/>
+      <c r="U34" s="7"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3109,8 +3195,10 @@
       <c r="S35" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T35" s="5"/>
+      <c r="U35" s="7"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3153,8 +3241,10 @@
       <c r="S36" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T36" s="5"/>
+      <c r="U36" s="7"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3194,8 +3284,10 @@
       <c r="S37" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T37" s="5"/>
+      <c r="U37" s="7"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3238,8 +3330,10 @@
       <c r="S38" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T38" s="5"/>
+      <c r="U38" s="7"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3282,8 +3376,10 @@
       <c r="S39" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T39" s="5"/>
+      <c r="U39" s="7"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3324,11 +3420,14 @@
         <v>1</v>
       </c>
       <c r="S40" s="3"/>
-      <c r="T40" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T40" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="U40" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3366,10 +3465,12 @@
         <v>0</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+      <c r="T41" s="5"/>
+      <c r="U41" s="7"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3412,8 +3513,10 @@
       <c r="S42" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T42" s="5"/>
+      <c r="U42" s="7"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3462,8 +3565,10 @@
       <c r="S43" s="3" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T43" s="5"/>
+      <c r="U43" s="7"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3506,8 +3611,10 @@
       <c r="S44" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T44" s="5"/>
+      <c r="U44" s="7"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3550,8 +3657,10 @@
       <c r="S45" s="3" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T45" s="5"/>
+      <c r="U45" s="7"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3594,56 +3703,61 @@
       <c r="S46" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
+      <c r="T46" s="5"/>
+      <c r="U46" s="7"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
         <v>45</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <v>2018</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="6">
         <v>3</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G47" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="H47" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7" t="s">
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P47" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q47" s="7"/>
-      <c r="R47" s="7">
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6">
         <v>1</v>
       </c>
-      <c r="S47" s="7"/>
-      <c r="T47" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S47" s="6"/>
+      <c r="T47" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="U47" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3686,8 +3800,10 @@
       <c r="S48" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T48" s="5"/>
+      <c r="U48" s="7"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3730,8 +3846,10 @@
       <c r="S49" s="3" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T49" s="5"/>
+      <c r="U49" s="7"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3777,8 +3895,10 @@
       <c r="S50" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T50" s="5"/>
+      <c r="U50" s="7"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3821,8 +3941,10 @@
       <c r="S51" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T51" s="5"/>
+      <c r="U51" s="7"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3868,8 +3990,10 @@
       <c r="S52" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T52" s="5"/>
+      <c r="U52" s="7"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3915,8 +4039,10 @@
       <c r="S53" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T53" s="5"/>
+      <c r="U53" s="7"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3965,8 +4091,10 @@
       <c r="S54" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T54" s="5"/>
+      <c r="U54" s="7"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4009,8 +4137,10 @@
       <c r="S55" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T55" s="5"/>
+      <c r="U55" s="7"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4050,8 +4180,10 @@
       <c r="S56" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T56" s="5"/>
+      <c r="U56" s="7"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4094,8 +4226,10 @@
       <c r="S57" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T57" s="5"/>
+      <c r="U57" s="7"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4138,8 +4272,10 @@
       <c r="S58" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T58" s="5"/>
+      <c r="U58" s="7"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4182,55 +4318,60 @@
       <c r="S59" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A60" s="7">
+      <c r="T59" s="5"/>
+      <c r="U59" s="7"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
         <v>58</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="6">
         <v>2021</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F60" s="6">
         <v>61</v>
       </c>
-      <c r="G60" s="7" t="s">
+      <c r="G60" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H60" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I60" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7" t="s">
+      <c r="J60" s="6"/>
+      <c r="K60" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P60" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q60" s="7"/>
-      <c r="R60" s="7">
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P60" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6">
         <v>1</v>
       </c>
-      <c r="S60" s="7"/>
-      <c r="T60" s="7" t="s">
-        <v>367</v>
+      <c r="S60" s="6"/>
+      <c r="T60" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="U60" s="7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>